<commit_message>
refactor(invoicing): SAV-1028: Added 'category' column to InvoiceProduct
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">sourceRecordId</t>
   </si>
   <si>
-    <t xml:space="preserve">sourceRecordType</t>
+    <t xml:space="preserve">category</t>
   </si>
   <si>
     <t xml:space="preserve">discountable</t>
@@ -172,10 +172,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>

</xml_diff>

<commit_message>
fix(referenceData): SAV-1059: Updated unit tests
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvoiceProduct-cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -149,6 +158,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +185,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>
@@ -225,6 +238,23 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(referenceData): SAV-1059: Fix missing error stats in import/export of reference data (#8721)
* fix(referenceData): SAV-1059: Fix missing error stats in import/export of ref data

* fix(referenceData): SAV-1059: Updated unit tests

* fix(referenceData): SAV-1059: Updated errors for InvoicePriceListItems

* Delete file as it was an exact duplicate of invoicePriceListLoader.test.js

* Update missed spots from new code

---------

Co-authored-by: Rohan Port <rohan@bes.au>
Co-authored-by: Emilio Navarro <DevNavarroEmilioLuis@gmail.com>
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-invalid-invoice-product-missing-source.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvoiceProduct-cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -149,6 +158,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +185,10 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24"/>
@@ -225,6 +238,23 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>